<commit_message>
test for PB01 + PB11
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\K21T2-CAP\Project\Source code\TrangTuyenDung.UITests.Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PB05_Login" sheetId="1" r:id="rId1"/>
+    <sheet name="PB01_CreateStaffAccount" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Email</t>
   </si>
@@ -42,6 +43,18 @@
   </si>
   <si>
     <t>P1%</t>
+  </si>
+  <si>
+    <t>admin@gmail.com</t>
+  </si>
+  <si>
+    <t>StaffAccountTest@gmail.com</t>
+  </si>
+  <si>
+    <t>Email Created</t>
+  </si>
+  <si>
+    <t>Password Created</t>
   </si>
 </sst>
 </file>
@@ -370,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,11 +427,58 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>1234567890</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
search recruitment news (all + city)
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PB05_Login" sheetId="1" r:id="rId1"/>
     <sheet name="PB01_CreateStaffAccount" sheetId="2" r:id="rId2"/>
+    <sheet name="PB12_SearchRN" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Email</t>
   </si>
@@ -55,6 +56,18 @@
   </si>
   <si>
     <t>Password Created</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input free data </t>
+  </si>
+  <si>
+    <t>Lập trình</t>
   </si>
 </sst>
 </file>
@@ -450,7 +463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -482,4 +495,38 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>